<commit_message>
add index with value order
</commit_message>
<xml_diff>
--- a/input/Financial Statement MSFT/Compiled Income Statement-MSFT.xlsx
+++ b/input/Financial Statement MSFT/Compiled Income Statement-MSFT.xlsx
@@ -929,28 +929,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>total cost of revenue</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>34261</v>
-      </c>
-      <c r="C9" t="n">
-        <v>8278</v>
-      </c>
-      <c r="D9" t="n">
-        <v>11064</v>
-      </c>
-      <c r="E9" t="n">
-        <v>9269</v>
-      </c>
+          <t>restructuring</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
@@ -970,412 +964,418 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>gross margin</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>55689</v>
-      </c>
-      <c r="C10" t="n">
-        <v>16260</v>
-      </c>
-      <c r="D10" t="n">
-        <v>17854</v>
-      </c>
-      <c r="E10" t="n">
-        <v>17550</v>
-      </c>
-      <c r="F10" t="n">
-        <v>54457</v>
-      </c>
+          <t>impairment and restructuring</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="n">
-        <v>72007</v>
-      </c>
-      <c r="H10" t="n">
-        <v>19179</v>
-      </c>
-      <c r="I10" t="n">
-        <v>20048</v>
-      </c>
-      <c r="J10" t="n">
-        <v>20401</v>
-      </c>
-      <c r="K10" t="n">
-        <v>62532</v>
-      </c>
-      <c r="L10" t="n">
-        <v>82933</v>
-      </c>
-      <c r="M10" t="n">
-        <v>22649</v>
-      </c>
-      <c r="N10" t="n">
-        <v>24548</v>
-      </c>
-      <c r="O10" t="n">
-        <v>24046</v>
-      </c>
-      <c r="P10" t="n">
-        <v>72891</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>96937</v>
-      </c>
-      <c r="R10" t="n">
-        <v>26152</v>
-      </c>
-      <c r="S10" t="n">
-        <v>28882</v>
-      </c>
-      <c r="T10" t="n">
-        <v>28661</v>
-      </c>
-      <c r="U10" t="n">
-        <v>87195</v>
-      </c>
-      <c r="V10" t="n">
-        <v>115856</v>
-      </c>
-      <c r="W10" t="n">
-        <v>31671</v>
-      </c>
-      <c r="X10" t="n">
-        <v>34768</v>
-      </c>
-      <c r="Y10" t="n">
-        <v>33745</v>
-      </c>
-      <c r="Z10" t="n">
-        <v>101875</v>
-      </c>
-      <c r="AA10" t="n">
-        <v>135620</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr"/>
+      <c r="AA10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>research and development</t>
+          <t>total cost of revenue</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>13037</v>
+        <v>34261</v>
       </c>
       <c r="C11" t="n">
-        <v>3574</v>
+        <v>8278</v>
       </c>
       <c r="D11" t="n">
-        <v>3504</v>
+        <v>11064</v>
       </c>
       <c r="E11" t="n">
-        <v>3715</v>
-      </c>
-      <c r="F11" t="n">
-        <v>11011</v>
-      </c>
-      <c r="G11" t="n">
-        <v>14726</v>
-      </c>
-      <c r="H11" t="n">
-        <v>3977</v>
-      </c>
-      <c r="I11" t="n">
-        <v>4070</v>
-      </c>
-      <c r="J11" t="n">
-        <v>4316</v>
-      </c>
-      <c r="K11" t="n">
-        <v>12560</v>
-      </c>
-      <c r="L11" t="n">
-        <v>16876</v>
-      </c>
-      <c r="M11" t="n">
-        <v>4565</v>
-      </c>
-      <c r="N11" t="n">
-        <v>4603</v>
-      </c>
-      <c r="O11" t="n">
-        <v>4887</v>
-      </c>
-      <c r="P11" t="n">
-        <v>14382</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>19269</v>
-      </c>
-      <c r="R11" t="n">
-        <v>4926</v>
-      </c>
-      <c r="S11" t="n">
-        <v>4899</v>
-      </c>
-      <c r="T11" t="n">
-        <v>5204</v>
-      </c>
-      <c r="U11" t="n">
-        <v>15512</v>
-      </c>
-      <c r="V11" t="n">
-        <v>20716</v>
-      </c>
-      <c r="W11" t="n">
-        <v>5599</v>
-      </c>
-      <c r="X11" t="n">
-        <v>5758</v>
-      </c>
-      <c r="Y11" t="n">
-        <v>6306</v>
-      </c>
-      <c r="Z11" t="n">
-        <v>18206</v>
-      </c>
-      <c r="AA11" t="n">
-        <v>24512</v>
-      </c>
+        <v>9269</v>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
+      <c r="X11" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
+      <c r="Z11" t="inlineStr"/>
+      <c r="AA11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>sales and marketing</t>
+          <t>gross margin</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>15539</v>
+        <v>55689</v>
       </c>
       <c r="C12" t="n">
-        <v>3812</v>
+        <v>16260</v>
       </c>
       <c r="D12" t="n">
-        <v>4562</v>
+        <v>17854</v>
       </c>
       <c r="E12" t="n">
-        <v>4335</v>
+        <v>17550</v>
       </c>
       <c r="F12" t="n">
-        <v>13134</v>
+        <v>54457</v>
       </c>
       <c r="G12" t="n">
-        <v>17469</v>
+        <v>72007</v>
       </c>
       <c r="H12" t="n">
-        <v>4098</v>
+        <v>19179</v>
       </c>
       <c r="I12" t="n">
-        <v>4588</v>
+        <v>20048</v>
       </c>
       <c r="J12" t="n">
-        <v>4565</v>
+        <v>20401</v>
       </c>
       <c r="K12" t="n">
-        <v>13648</v>
+        <v>62532</v>
       </c>
       <c r="L12" t="n">
-        <v>18213</v>
+        <v>82933</v>
       </c>
       <c r="M12" t="n">
-        <v>4337</v>
+        <v>22649</v>
       </c>
       <c r="N12" t="n">
-        <v>4933</v>
+        <v>24548</v>
       </c>
       <c r="O12" t="n">
-        <v>4911</v>
+        <v>24046</v>
       </c>
       <c r="P12" t="n">
-        <v>14687</v>
+        <v>72891</v>
       </c>
       <c r="Q12" t="n">
-        <v>19598</v>
+        <v>96937</v>
       </c>
       <c r="R12" t="n">
-        <v>4231</v>
+        <v>26152</v>
       </c>
       <c r="S12" t="n">
-        <v>4947</v>
+        <v>28882</v>
       </c>
       <c r="T12" t="n">
-        <v>5082</v>
+        <v>28661</v>
       </c>
       <c r="U12" t="n">
-        <v>15035</v>
+        <v>87195</v>
       </c>
       <c r="V12" t="n">
-        <v>20117</v>
+        <v>115856</v>
       </c>
       <c r="W12" t="n">
-        <v>4547</v>
+        <v>31671</v>
       </c>
       <c r="X12" t="n">
-        <v>5379</v>
+        <v>34768</v>
       </c>
       <c r="Y12" t="n">
-        <v>5595</v>
+        <v>33745</v>
       </c>
       <c r="Z12" t="n">
-        <v>16230</v>
+        <v>101875</v>
       </c>
       <c r="AA12" t="n">
-        <v>21825</v>
+        <v>135620</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>general and administrative</t>
+          <t>research and development</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>4481</v>
+        <v>13037</v>
       </c>
       <c r="C13" t="n">
-        <v>1166</v>
+        <v>3574</v>
       </c>
       <c r="D13" t="n">
-        <v>1109</v>
+        <v>3504</v>
       </c>
       <c r="E13" t="n">
-        <v>1208</v>
+        <v>3715</v>
       </c>
       <c r="F13" t="n">
-        <v>3546</v>
+        <v>11011</v>
       </c>
       <c r="G13" t="n">
-        <v>4754</v>
+        <v>14726</v>
       </c>
       <c r="H13" t="n">
-        <v>1149</v>
+        <v>3977</v>
       </c>
       <c r="I13" t="n">
-        <v>1132</v>
+        <v>4070</v>
       </c>
       <c r="J13" t="n">
-        <v>1179</v>
+        <v>4316</v>
       </c>
       <c r="K13" t="n">
-        <v>3706</v>
+        <v>12560</v>
       </c>
       <c r="L13" t="n">
-        <v>4885</v>
+        <v>16876</v>
       </c>
       <c r="M13" t="n">
-        <v>1061</v>
+        <v>4565</v>
       </c>
       <c r="N13" t="n">
-        <v>1121</v>
+        <v>4603</v>
       </c>
       <c r="O13" t="n">
-        <v>1273</v>
+        <v>4887</v>
       </c>
       <c r="P13" t="n">
-        <v>3838</v>
+        <v>14382</v>
       </c>
       <c r="Q13" t="n">
-        <v>5111</v>
+        <v>19269</v>
       </c>
       <c r="R13" t="n">
-        <v>1119</v>
+        <v>4926</v>
       </c>
       <c r="S13" t="n">
-        <v>1139</v>
+        <v>4899</v>
       </c>
       <c r="T13" t="n">
-        <v>1327</v>
+        <v>5204</v>
       </c>
       <c r="U13" t="n">
-        <v>3780</v>
+        <v>15512</v>
       </c>
       <c r="V13" t="n">
-        <v>5107</v>
+        <v>20716</v>
       </c>
       <c r="W13" t="n">
-        <v>1287</v>
+        <v>5599</v>
       </c>
       <c r="X13" t="n">
-        <v>1384</v>
+        <v>5758</v>
       </c>
       <c r="Y13" t="n">
-        <v>1480</v>
+        <v>6306</v>
       </c>
       <c r="Z13" t="n">
-        <v>4420</v>
+        <v>18206</v>
       </c>
       <c r="AA13" t="n">
-        <v>5900</v>
+        <v>24512</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>restructuring</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
+          <t>sales and marketing</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>15539</v>
+      </c>
+      <c r="C14" t="n">
+        <v>3812</v>
+      </c>
+      <c r="D14" t="n">
+        <v>4562</v>
+      </c>
+      <c r="E14" t="n">
+        <v>4335</v>
+      </c>
+      <c r="F14" t="n">
+        <v>13134</v>
+      </c>
+      <c r="G14" t="n">
+        <v>17469</v>
+      </c>
+      <c r="H14" t="n">
+        <v>4098</v>
+      </c>
+      <c r="I14" t="n">
+        <v>4588</v>
+      </c>
+      <c r="J14" t="n">
+        <v>4565</v>
+      </c>
+      <c r="K14" t="n">
+        <v>13648</v>
+      </c>
       <c r="L14" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
-      <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr"/>
-      <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr"/>
-      <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="inlineStr"/>
-      <c r="Z14" t="inlineStr"/>
-      <c r="AA14" t="inlineStr"/>
+        <v>18213</v>
+      </c>
+      <c r="M14" t="n">
+        <v>4337</v>
+      </c>
+      <c r="N14" t="n">
+        <v>4933</v>
+      </c>
+      <c r="O14" t="n">
+        <v>4911</v>
+      </c>
+      <c r="P14" t="n">
+        <v>14687</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>19598</v>
+      </c>
+      <c r="R14" t="n">
+        <v>4231</v>
+      </c>
+      <c r="S14" t="n">
+        <v>4947</v>
+      </c>
+      <c r="T14" t="n">
+        <v>5082</v>
+      </c>
+      <c r="U14" t="n">
+        <v>15035</v>
+      </c>
+      <c r="V14" t="n">
+        <v>20117</v>
+      </c>
+      <c r="W14" t="n">
+        <v>4547</v>
+      </c>
+      <c r="X14" t="n">
+        <v>5379</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>5595</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>16230</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>21825</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>impairment and restructuring</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
+          <t>general and administrative</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>4481</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1166</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1109</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1208</v>
+      </c>
+      <c r="F15" t="n">
+        <v>3546</v>
+      </c>
       <c r="G15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
-      <c r="T15" t="inlineStr"/>
-      <c r="U15" t="inlineStr"/>
-      <c r="V15" t="inlineStr"/>
-      <c r="W15" t="inlineStr"/>
-      <c r="X15" t="inlineStr"/>
-      <c r="Y15" t="inlineStr"/>
-      <c r="Z15" t="inlineStr"/>
-      <c r="AA15" t="inlineStr"/>
+        <v>4754</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1149</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1132</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1179</v>
+      </c>
+      <c r="K15" t="n">
+        <v>3706</v>
+      </c>
+      <c r="L15" t="n">
+        <v>4885</v>
+      </c>
+      <c r="M15" t="n">
+        <v>1061</v>
+      </c>
+      <c r="N15" t="n">
+        <v>1121</v>
+      </c>
+      <c r="O15" t="n">
+        <v>1273</v>
+      </c>
+      <c r="P15" t="n">
+        <v>3838</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>5111</v>
+      </c>
+      <c r="R15" t="n">
+        <v>1119</v>
+      </c>
+      <c r="S15" t="n">
+        <v>1139</v>
+      </c>
+      <c r="T15" t="n">
+        <v>1327</v>
+      </c>
+      <c r="U15" t="n">
+        <v>3780</v>
+      </c>
+      <c r="V15" t="n">
+        <v>5107</v>
+      </c>
+      <c r="W15" t="n">
+        <v>1287</v>
+      </c>
+      <c r="X15" t="n">
+        <v>1384</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>1480</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>4420</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>5900</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1415,153 +1415,153 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>operating income</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>22326</v>
-      </c>
+          <t>other income, net</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
       <c r="C17" t="n">
-        <v>7708</v>
+        <v>276</v>
       </c>
       <c r="D17" t="n">
-        <v>8679</v>
+        <v>490</v>
       </c>
       <c r="E17" t="n">
-        <v>8292</v>
-      </c>
-      <c r="F17" t="n">
-        <v>26766</v>
-      </c>
-      <c r="G17" t="n">
-        <v>35058</v>
-      </c>
+        <v>349</v>
+      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
       <c r="H17" t="n">
-        <v>9955</v>
+        <v>266</v>
       </c>
       <c r="I17" t="n">
-        <v>10258</v>
+        <v>127</v>
       </c>
       <c r="J17" t="n">
-        <v>10341</v>
+        <v>145</v>
       </c>
       <c r="K17" t="n">
-        <v>32618</v>
+        <v>584</v>
       </c>
       <c r="L17" t="n">
-        <v>42959</v>
+        <v>729</v>
       </c>
       <c r="M17" t="n">
-        <v>12686</v>
+        <v>0</v>
       </c>
       <c r="N17" t="n">
-        <v>13891</v>
-      </c>
-      <c r="O17" t="n">
-        <v>12975</v>
-      </c>
-      <c r="P17" t="n">
-        <v>39984</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
       <c r="Q17" t="n">
-        <v>52959</v>
+        <v>77</v>
       </c>
       <c r="R17" t="n">
-        <v>15876</v>
+        <v>248</v>
       </c>
       <c r="S17" t="n">
-        <v>17897</v>
-      </c>
-      <c r="T17" t="n">
-        <v>17048</v>
-      </c>
-      <c r="U17" t="n">
-        <v>52868</v>
-      </c>
+        <v>440</v>
+      </c>
+      <c r="T17" t="inlineStr"/>
+      <c r="U17" t="inlineStr"/>
       <c r="V17" t="n">
-        <v>69916</v>
+        <v>1186</v>
       </c>
       <c r="W17" t="n">
-        <v>20238</v>
+        <v>286</v>
       </c>
       <c r="X17" t="n">
-        <v>22247</v>
-      </c>
-      <c r="Y17" t="n">
-        <v>20364</v>
-      </c>
-      <c r="Z17" t="n">
-        <v>63019</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="Y17" t="inlineStr"/>
+      <c r="Z17" t="inlineStr"/>
       <c r="AA17" t="n">
-        <v>83383</v>
+        <v>333</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>other income, net</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
+          <t>operating income</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>22326</v>
+      </c>
       <c r="C18" t="n">
-        <v>276</v>
+        <v>7708</v>
       </c>
       <c r="D18" t="n">
-        <v>490</v>
+        <v>8679</v>
       </c>
       <c r="E18" t="n">
-        <v>349</v>
-      </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
+        <v>8292</v>
+      </c>
+      <c r="F18" t="n">
+        <v>26766</v>
+      </c>
+      <c r="G18" t="n">
+        <v>35058</v>
+      </c>
       <c r="H18" t="n">
-        <v>266</v>
+        <v>9955</v>
       </c>
       <c r="I18" t="n">
-        <v>127</v>
+        <v>10258</v>
       </c>
       <c r="J18" t="n">
-        <v>145</v>
+        <v>10341</v>
       </c>
       <c r="K18" t="n">
-        <v>584</v>
+        <v>32618</v>
       </c>
       <c r="L18" t="n">
-        <v>729</v>
+        <v>42959</v>
       </c>
       <c r="M18" t="n">
-        <v>0</v>
+        <v>12686</v>
       </c>
       <c r="N18" t="n">
-        <v>194</v>
-      </c>
-      <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr"/>
+        <v>13891</v>
+      </c>
+      <c r="O18" t="n">
+        <v>12975</v>
+      </c>
+      <c r="P18" t="n">
+        <v>39984</v>
+      </c>
       <c r="Q18" t="n">
-        <v>77</v>
+        <v>52959</v>
       </c>
       <c r="R18" t="n">
-        <v>248</v>
+        <v>15876</v>
       </c>
       <c r="S18" t="n">
-        <v>440</v>
-      </c>
-      <c r="T18" t="inlineStr"/>
-      <c r="U18" t="inlineStr"/>
+        <v>17897</v>
+      </c>
+      <c r="T18" t="n">
+        <v>17048</v>
+      </c>
+      <c r="U18" t="n">
+        <v>52868</v>
+      </c>
       <c r="V18" t="n">
-        <v>1186</v>
+        <v>69916</v>
       </c>
       <c r="W18" t="n">
-        <v>286</v>
+        <v>20238</v>
       </c>
       <c r="X18" t="n">
-        <v>268</v>
-      </c>
-      <c r="Y18" t="inlineStr"/>
-      <c r="Z18" t="inlineStr"/>
+        <v>22247</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>20364</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>63019</v>
+      </c>
       <c r="AA18" t="n">
-        <v>333</v>
+        <v>83383</v>
       </c>
     </row>
     <row r="19">
@@ -1987,383 +1987,401 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>diluted</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>2.71</v>
-      </c>
-      <c r="C25" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="D25" t="n">
-        <v>-0.82</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="F25" t="n">
-        <v>1.18</v>
-      </c>
-      <c r="G25" t="n">
-        <v>2.13</v>
-      </c>
-      <c r="H25" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="I25" t="n">
-        <v>1.08</v>
-      </c>
-      <c r="J25" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="K25" t="n">
-        <v>3.92</v>
-      </c>
-      <c r="L25" t="n">
-        <v>5.06</v>
-      </c>
-      <c r="M25" t="n">
-        <v>1.38</v>
-      </c>
-      <c r="N25" t="n">
-        <v>1.51</v>
-      </c>
-      <c r="O25" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="P25" t="n">
-        <v>4.359999999999999</v>
-      </c>
-      <c r="Q25" t="n">
-        <v>5.76</v>
-      </c>
-      <c r="R25" t="n">
-        <v>1.82</v>
-      </c>
-      <c r="S25" t="n">
-        <v>2.03</v>
-      </c>
-      <c r="T25" t="n">
-        <v>2.03</v>
-      </c>
-      <c r="U25" t="n">
-        <v>6.020000000000001</v>
-      </c>
-      <c r="V25" t="n">
-        <v>8.050000000000001</v>
-      </c>
-      <c r="W25" t="n">
-        <v>2.71</v>
-      </c>
-      <c r="X25" t="n">
-        <v>2.48</v>
-      </c>
-      <c r="Y25" t="n">
-        <v>2.22</v>
-      </c>
-      <c r="Z25" t="n">
-        <v>7.43</v>
-      </c>
-      <c r="AA25" t="n">
-        <v>9.65</v>
+          <t>product</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr"/>
+      <c r="R25" t="inlineStr"/>
+      <c r="S25" t="inlineStr"/>
+      <c r="T25" t="inlineStr"/>
+      <c r="U25" t="inlineStr"/>
+      <c r="V25" t="inlineStr"/>
+      <c r="W25" t="inlineStr"/>
+      <c r="X25" t="inlineStr"/>
+      <c r="Y25" t="inlineStr"/>
+      <c r="Z25" t="inlineStr"/>
+      <c r="AA25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>weighted average shares outstanding:</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="inlineStr"/>
-      <c r="N26" t="inlineStr"/>
-      <c r="O26" t="inlineStr"/>
-      <c r="P26" t="inlineStr"/>
-      <c r="Q26" t="inlineStr"/>
-      <c r="R26" t="inlineStr"/>
-      <c r="S26" t="inlineStr"/>
-      <c r="T26" t="inlineStr"/>
-      <c r="U26" t="inlineStr"/>
-      <c r="V26" t="inlineStr"/>
-      <c r="W26" t="inlineStr"/>
-      <c r="X26" t="inlineStr"/>
-      <c r="Y26" t="inlineStr"/>
-      <c r="Z26" t="inlineStr"/>
-      <c r="AA26" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+          <t>diluted</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>2.71</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="D26" t="n">
+        <v>-0.82</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="G26" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="I26" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="J26" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="K26" t="n">
+        <v>3.92</v>
+      </c>
+      <c r="L26" t="n">
+        <v>5.06</v>
+      </c>
+      <c r="M26" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="N26" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="O26" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="P26" t="n">
+        <v>4.359999999999999</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>5.76</v>
+      </c>
+      <c r="R26" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="S26" t="n">
+        <v>2.03</v>
+      </c>
+      <c r="T26" t="n">
+        <v>2.03</v>
+      </c>
+      <c r="U26" t="n">
+        <v>6.020000000000001</v>
+      </c>
+      <c r="V26" t="n">
+        <v>8.050000000000001</v>
+      </c>
+      <c r="W26" t="n">
+        <v>2.71</v>
+      </c>
+      <c r="X26" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>7.43</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>9.65</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>basic</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>7746</v>
-      </c>
-      <c r="C27" t="n">
-        <v>7708</v>
-      </c>
-      <c r="D27" t="n">
-        <v>7710</v>
-      </c>
-      <c r="E27" t="n">
-        <v>7698</v>
-      </c>
-      <c r="F27" t="n">
-        <v>2</v>
-      </c>
+          <t>revenue</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
       <c r="G27" t="n">
-        <v>7700</v>
+        <v>64497</v>
       </c>
       <c r="H27" t="n">
-        <v>7673</v>
+        <v>17299</v>
       </c>
       <c r="I27" t="n">
-        <v>7692</v>
+        <v>16219</v>
       </c>
       <c r="J27" t="n">
-        <v>7672</v>
+        <v>15448</v>
       </c>
       <c r="K27" t="n">
-        <v>1</v>
+        <v>50621</v>
       </c>
       <c r="L27" t="n">
-        <v>7673</v>
+        <v>66069</v>
       </c>
       <c r="M27" t="n">
-        <v>7634</v>
+        <v>15768</v>
       </c>
       <c r="N27" t="n">
-        <v>7621</v>
+        <v>18255</v>
       </c>
       <c r="O27" t="n">
-        <v>7602</v>
+        <v>15871</v>
       </c>
       <c r="P27" t="n">
-        <v>8</v>
+        <v>52170</v>
       </c>
       <c r="Q27" t="n">
-        <v>7610</v>
+        <v>68041</v>
       </c>
       <c r="R27" t="n">
-        <v>7566</v>
+        <v>15803</v>
       </c>
       <c r="S27" t="n">
-        <v>7555</v>
+        <v>19460</v>
       </c>
       <c r="T27" t="n">
-        <v>7539</v>
+        <v>16873</v>
       </c>
       <c r="U27" t="n">
-        <v>8</v>
+        <v>54201</v>
       </c>
       <c r="V27" t="n">
-        <v>7547</v>
+        <v>71074</v>
       </c>
       <c r="W27" t="n">
-        <v>7513</v>
+        <v>16631</v>
       </c>
       <c r="X27" t="n">
-        <v>7505</v>
+        <v>20779</v>
       </c>
       <c r="Y27" t="n">
-        <v>7493</v>
+        <v>17366</v>
       </c>
       <c r="Z27" t="n">
-        <v>3</v>
+        <v>55366</v>
       </c>
       <c r="AA27" t="n">
-        <v>7496</v>
+        <v>72732</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>diluted</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>7832</v>
-      </c>
-      <c r="C28" t="n">
-        <v>7799</v>
-      </c>
-      <c r="D28" t="n">
-        <v>7710</v>
-      </c>
-      <c r="E28" t="n">
-        <v>7794</v>
-      </c>
-      <c r="F28" t="n">
-        <v>0</v>
-      </c>
-      <c r="G28" t="n">
-        <v>7794</v>
-      </c>
-      <c r="H28" t="n">
-        <v>7766</v>
-      </c>
-      <c r="I28" t="n">
-        <v>7768</v>
-      </c>
-      <c r="J28" t="n">
-        <v>7744</v>
-      </c>
-      <c r="K28" t="n">
-        <v>9</v>
-      </c>
-      <c r="L28" t="n">
-        <v>7753</v>
-      </c>
-      <c r="M28" t="n">
-        <v>7710</v>
-      </c>
-      <c r="N28" t="n">
-        <v>7691</v>
-      </c>
-      <c r="O28" t="n">
-        <v>7675</v>
-      </c>
-      <c r="P28" t="n">
-        <v>8</v>
-      </c>
-      <c r="Q28" t="n">
-        <v>7683</v>
-      </c>
-      <c r="R28" t="n">
-        <v>7637</v>
-      </c>
-      <c r="S28" t="n">
-        <v>7616</v>
-      </c>
-      <c r="T28" t="n">
-        <v>7597</v>
-      </c>
-      <c r="U28" t="n">
-        <v>11</v>
-      </c>
-      <c r="V28" t="n">
-        <v>7608</v>
-      </c>
-      <c r="W28" t="n">
-        <v>7567</v>
-      </c>
-      <c r="X28" t="n">
-        <v>7555</v>
-      </c>
-      <c r="Y28" t="n">
-        <v>7534</v>
-      </c>
-      <c r="Z28" t="n">
-        <v>6</v>
-      </c>
-      <c r="AA28" t="n">
-        <v>7540</v>
+          <t>weighted average shares outstanding:</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr"/>
+      <c r="R28" t="inlineStr"/>
+      <c r="S28" t="inlineStr"/>
+      <c r="T28" t="inlineStr"/>
+      <c r="U28" t="inlineStr"/>
+      <c r="V28" t="inlineStr"/>
+      <c r="W28" t="inlineStr"/>
+      <c r="X28" t="inlineStr"/>
+      <c r="Y28" t="inlineStr"/>
+      <c r="Z28" t="inlineStr"/>
+      <c r="AA28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>cash dividends declared per common share</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>1.56</v>
-      </c>
-      <c r="C29" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="D29" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="E29" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="F29" t="n">
-        <v>1.26</v>
-      </c>
+          <t>cost of revenue</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
       <c r="G29" t="n">
-        <v>1.68</v>
+        <v>15420</v>
       </c>
       <c r="H29" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
-      <c r="K29" t="inlineStr"/>
-      <c r="L29" t="inlineStr"/>
-      <c r="M29" t="inlineStr"/>
-      <c r="N29" t="inlineStr"/>
-      <c r="O29" t="inlineStr"/>
-      <c r="P29" t="inlineStr"/>
-      <c r="Q29" t="inlineStr"/>
-      <c r="R29" t="inlineStr"/>
-      <c r="S29" t="inlineStr"/>
-      <c r="T29" t="inlineStr"/>
-      <c r="U29" t="inlineStr"/>
-      <c r="V29" t="inlineStr"/>
-      <c r="W29" t="inlineStr"/>
-      <c r="X29" t="inlineStr"/>
-      <c r="Y29" t="inlineStr"/>
-      <c r="Z29" t="inlineStr"/>
-      <c r="AA29" t="inlineStr"/>
+        <v>3649</v>
+      </c>
+      <c r="I29" t="n">
+        <v>5885</v>
+      </c>
+      <c r="J29" t="n">
+        <v>3441</v>
+      </c>
+      <c r="K29" t="n">
+        <v>12832</v>
+      </c>
+      <c r="L29" t="n">
+        <v>16273</v>
+      </c>
+      <c r="M29" t="n">
+        <v>3305</v>
+      </c>
+      <c r="N29" t="n">
+        <v>4966</v>
+      </c>
+      <c r="O29" t="n">
+        <v>3376</v>
+      </c>
+      <c r="P29" t="n">
+        <v>12641</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>16017</v>
+      </c>
+      <c r="R29" t="n">
+        <v>3597</v>
+      </c>
+      <c r="S29" t="n">
+        <v>6058</v>
+      </c>
+      <c r="T29" t="n">
+        <v>4277</v>
+      </c>
+      <c r="U29" t="n">
+        <v>13942</v>
+      </c>
+      <c r="V29" t="n">
+        <v>18219</v>
+      </c>
+      <c r="W29" t="n">
+        <v>3792</v>
+      </c>
+      <c r="X29" t="n">
+        <v>6331</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>4584</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>14480</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>19064</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>product</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr"/>
-      <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr"/>
-      <c r="J30" t="inlineStr"/>
-      <c r="K30" t="inlineStr"/>
-      <c r="L30" t="inlineStr"/>
-      <c r="M30" t="inlineStr"/>
-      <c r="N30" t="inlineStr"/>
-      <c r="O30" t="inlineStr"/>
-      <c r="P30" t="inlineStr"/>
-      <c r="Q30" t="inlineStr"/>
-      <c r="R30" t="inlineStr"/>
-      <c r="S30" t="inlineStr"/>
-      <c r="T30" t="inlineStr"/>
-      <c r="U30" t="inlineStr"/>
-      <c r="V30" t="inlineStr"/>
-      <c r="W30" t="inlineStr"/>
-      <c r="X30" t="inlineStr"/>
-      <c r="Y30" t="inlineStr"/>
-      <c r="Z30" t="inlineStr"/>
-      <c r="AA30" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+          <t>basic</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>7746</v>
+      </c>
+      <c r="C30" t="n">
+        <v>7708</v>
+      </c>
+      <c r="D30" t="n">
+        <v>7710</v>
+      </c>
+      <c r="E30" t="n">
+        <v>7698</v>
+      </c>
+      <c r="F30" t="n">
+        <v>2</v>
+      </c>
+      <c r="G30" t="n">
+        <v>7700</v>
+      </c>
+      <c r="H30" t="n">
+        <v>7673</v>
+      </c>
+      <c r="I30" t="n">
+        <v>7692</v>
+      </c>
+      <c r="J30" t="n">
+        <v>7672</v>
+      </c>
+      <c r="K30" t="n">
+        <v>1</v>
+      </c>
+      <c r="L30" t="n">
+        <v>7673</v>
+      </c>
+      <c r="M30" t="n">
+        <v>7634</v>
+      </c>
+      <c r="N30" t="n">
+        <v>7621</v>
+      </c>
+      <c r="O30" t="n">
+        <v>7602</v>
+      </c>
+      <c r="P30" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>7610</v>
+      </c>
+      <c r="R30" t="n">
+        <v>7566</v>
+      </c>
+      <c r="S30" t="n">
+        <v>7555</v>
+      </c>
+      <c r="T30" t="n">
+        <v>7539</v>
+      </c>
+      <c r="U30" t="n">
+        <v>8</v>
+      </c>
+      <c r="V30" t="n">
+        <v>7547</v>
+      </c>
+      <c r="W30" t="n">
+        <v>7513</v>
+      </c>
+      <c r="X30" t="n">
+        <v>7505</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>7493</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>7496</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>revenue</t>
+          <t>service and other</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -2371,74 +2389,36 @@
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
-      <c r="G31" t="n">
-        <v>64497</v>
-      </c>
-      <c r="H31" t="n">
-        <v>17299</v>
-      </c>
-      <c r="I31" t="n">
-        <v>16219</v>
-      </c>
-      <c r="J31" t="n">
-        <v>15448</v>
-      </c>
-      <c r="K31" t="n">
-        <v>50621</v>
-      </c>
-      <c r="L31" t="n">
-        <v>66069</v>
-      </c>
-      <c r="M31" t="n">
-        <v>15768</v>
-      </c>
-      <c r="N31" t="n">
-        <v>18255</v>
-      </c>
-      <c r="O31" t="n">
-        <v>15871</v>
-      </c>
-      <c r="P31" t="n">
-        <v>52170</v>
-      </c>
-      <c r="Q31" t="n">
-        <v>68041</v>
-      </c>
-      <c r="R31" t="n">
-        <v>15803</v>
-      </c>
-      <c r="S31" t="n">
-        <v>19460</v>
-      </c>
-      <c r="T31" t="n">
-        <v>16873</v>
-      </c>
-      <c r="U31" t="n">
-        <v>54201</v>
-      </c>
-      <c r="V31" t="n">
-        <v>71074</v>
-      </c>
-      <c r="W31" t="n">
-        <v>16631</v>
-      </c>
-      <c r="X31" t="n">
-        <v>20779</v>
-      </c>
-      <c r="Y31" t="n">
-        <v>17366</v>
-      </c>
-      <c r="Z31" t="n">
-        <v>55366</v>
-      </c>
-      <c r="AA31" t="n">
-        <v>72732</v>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr"/>
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
+      <c r="Q31" t="inlineStr"/>
+      <c r="R31" t="inlineStr"/>
+      <c r="S31" t="inlineStr"/>
+      <c r="T31" t="inlineStr"/>
+      <c r="U31" t="inlineStr"/>
+      <c r="V31" t="inlineStr"/>
+      <c r="W31" t="inlineStr"/>
+      <c r="X31" t="inlineStr"/>
+      <c r="Y31" t="inlineStr"/>
+      <c r="Z31" t="inlineStr"/>
+      <c r="AA31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>cost of revenue</t>
+          <t>revenue</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -2447,180 +2427,200 @@
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="n">
-        <v>15420</v>
+        <v>45863</v>
       </c>
       <c r="H32" t="n">
-        <v>3649</v>
+        <v>11785</v>
       </c>
       <c r="I32" t="n">
-        <v>5885</v>
+        <v>16252</v>
       </c>
       <c r="J32" t="n">
-        <v>3441</v>
+        <v>15123</v>
       </c>
       <c r="K32" t="n">
-        <v>12832</v>
+        <v>44651</v>
       </c>
       <c r="L32" t="n">
-        <v>16273</v>
+        <v>59774</v>
       </c>
       <c r="M32" t="n">
-        <v>3305</v>
+        <v>17287</v>
       </c>
       <c r="N32" t="n">
-        <v>4966</v>
+        <v>18651</v>
       </c>
       <c r="O32" t="n">
-        <v>3376</v>
+        <v>19150</v>
       </c>
       <c r="P32" t="n">
-        <v>12641</v>
+        <v>55824</v>
       </c>
       <c r="Q32" t="n">
-        <v>16017</v>
+        <v>74974</v>
       </c>
       <c r="R32" t="n">
-        <v>3597</v>
+        <v>21351</v>
       </c>
       <c r="S32" t="n">
-        <v>6058</v>
+        <v>23616</v>
       </c>
       <c r="T32" t="n">
-        <v>4277</v>
+        <v>24833</v>
       </c>
       <c r="U32" t="n">
-        <v>13942</v>
+        <v>72181</v>
       </c>
       <c r="V32" t="n">
-        <v>18219</v>
+        <v>97014</v>
       </c>
       <c r="W32" t="n">
-        <v>3792</v>
+        <v>28686</v>
       </c>
       <c r="X32" t="n">
-        <v>6331</v>
+        <v>30949</v>
       </c>
       <c r="Y32" t="n">
-        <v>4584</v>
+        <v>31994</v>
       </c>
       <c r="Z32" t="n">
-        <v>14480</v>
+        <v>93544</v>
       </c>
       <c r="AA32" t="n">
-        <v>19064</v>
+        <v>125538</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>service and other</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr"/>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr"/>
-      <c r="J33" t="inlineStr"/>
-      <c r="K33" t="inlineStr"/>
-      <c r="L33" t="inlineStr"/>
-      <c r="M33" t="inlineStr"/>
-      <c r="N33" t="inlineStr"/>
-      <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr"/>
-      <c r="Q33" t="inlineStr"/>
-      <c r="R33" t="inlineStr"/>
-      <c r="S33" t="inlineStr"/>
-      <c r="T33" t="inlineStr"/>
-      <c r="U33" t="inlineStr"/>
-      <c r="V33" t="inlineStr"/>
-      <c r="W33" t="inlineStr"/>
-      <c r="X33" t="inlineStr"/>
-      <c r="Y33" t="inlineStr"/>
-      <c r="Z33" t="inlineStr"/>
-      <c r="AA33" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+          <t>diluted</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>7832</v>
+      </c>
+      <c r="C33" t="n">
+        <v>7799</v>
+      </c>
+      <c r="D33" t="n">
+        <v>7710</v>
+      </c>
+      <c r="E33" t="n">
+        <v>7794</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>7794</v>
+      </c>
+      <c r="H33" t="n">
+        <v>7766</v>
+      </c>
+      <c r="I33" t="n">
+        <v>7768</v>
+      </c>
+      <c r="J33" t="n">
+        <v>7744</v>
+      </c>
+      <c r="K33" t="n">
+        <v>9</v>
+      </c>
+      <c r="L33" t="n">
+        <v>7753</v>
+      </c>
+      <c r="M33" t="n">
+        <v>7710</v>
+      </c>
+      <c r="N33" t="n">
+        <v>7691</v>
+      </c>
+      <c r="O33" t="n">
+        <v>7675</v>
+      </c>
+      <c r="P33" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>7683</v>
+      </c>
+      <c r="R33" t="n">
+        <v>7637</v>
+      </c>
+      <c r="S33" t="n">
+        <v>7616</v>
+      </c>
+      <c r="T33" t="n">
+        <v>7597</v>
+      </c>
+      <c r="U33" t="n">
+        <v>11</v>
+      </c>
+      <c r="V33" t="n">
+        <v>7608</v>
+      </c>
+      <c r="W33" t="n">
+        <v>7567</v>
+      </c>
+      <c r="X33" t="n">
+        <v>7555</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>7534</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>6</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>7540</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>revenue</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr"/>
-      <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr"/>
-      <c r="F34" t="inlineStr"/>
+          <t>cash dividends declared per common share</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="F34" t="n">
+        <v>1.26</v>
+      </c>
       <c r="G34" t="n">
-        <v>45863</v>
+        <v>1.68</v>
       </c>
       <c r="H34" t="n">
-        <v>11785</v>
-      </c>
-      <c r="I34" t="n">
-        <v>16252</v>
-      </c>
-      <c r="J34" t="n">
-        <v>15123</v>
-      </c>
-      <c r="K34" t="n">
-        <v>44651</v>
-      </c>
-      <c r="L34" t="n">
-        <v>59774</v>
-      </c>
-      <c r="M34" t="n">
-        <v>17287</v>
-      </c>
-      <c r="N34" t="n">
-        <v>18651</v>
-      </c>
-      <c r="O34" t="n">
-        <v>19150</v>
-      </c>
-      <c r="P34" t="n">
-        <v>55824</v>
-      </c>
-      <c r="Q34" t="n">
-        <v>74974</v>
-      </c>
-      <c r="R34" t="n">
-        <v>21351</v>
-      </c>
-      <c r="S34" t="n">
-        <v>23616</v>
-      </c>
-      <c r="T34" t="n">
-        <v>24833</v>
-      </c>
-      <c r="U34" t="n">
-        <v>72181</v>
-      </c>
-      <c r="V34" t="n">
-        <v>97014</v>
-      </c>
-      <c r="W34" t="n">
-        <v>28686</v>
-      </c>
-      <c r="X34" t="n">
-        <v>30949</v>
-      </c>
-      <c r="Y34" t="n">
-        <v>31994</v>
-      </c>
-      <c r="Z34" t="n">
-        <v>93544</v>
-      </c>
-      <c r="AA34" t="n">
-        <v>125538</v>
-      </c>
+        <v>0.46</v>
+      </c>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
+      <c r="N34" t="inlineStr"/>
+      <c r="O34" t="inlineStr"/>
+      <c r="P34" t="inlineStr"/>
+      <c r="Q34" t="inlineStr"/>
+      <c r="R34" t="inlineStr"/>
+      <c r="S34" t="inlineStr"/>
+      <c r="T34" t="inlineStr"/>
+      <c r="U34" t="inlineStr"/>
+      <c r="V34" t="inlineStr"/>
+      <c r="W34" t="inlineStr"/>
+      <c r="X34" t="inlineStr"/>
+      <c r="Y34" t="inlineStr"/>
+      <c r="Z34" t="inlineStr"/>
+      <c r="AA34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3611,20 +3611,16 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>total cost of revenue</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>8278</v>
-      </c>
-      <c r="E9" t="n">
-        <v>11064</v>
-      </c>
-      <c r="F9" t="n">
-        <v>9269</v>
-      </c>
+          <t>impairment and restructuring</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
       <c r="I9" t="inlineStr">
         <is>
           <t>operating income</t>
@@ -3705,24 +3701,20 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>gross margin</t>
+          <t>total cost of revenue</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>16260</v>
+        <v>8278</v>
       </c>
       <c r="E10" t="n">
-        <v>17854</v>
+        <v>11064</v>
       </c>
       <c r="F10" t="n">
-        <v>17550</v>
-      </c>
-      <c r="G10" t="n">
-        <v>54457</v>
-      </c>
-      <c r="H10" t="n">
-        <v>72007</v>
-      </c>
+        <v>9269</v>
+      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr">
         <is>
           <t>other income, net</t>
@@ -3791,23 +3783,23 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>research and development</t>
+          <t>gross margin</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>3574</v>
+        <v>16260</v>
       </c>
       <c r="E11" t="n">
-        <v>3504</v>
+        <v>17854</v>
       </c>
       <c r="F11" t="n">
-        <v>3715</v>
+        <v>17550</v>
       </c>
       <c r="G11" t="n">
-        <v>11011</v>
+        <v>54457</v>
       </c>
       <c r="H11" t="n">
-        <v>14726</v>
+        <v>72007</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -3901,23 +3893,15 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>sales and marketing</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>3812</v>
-      </c>
-      <c r="E12" t="n">
-        <v>4562</v>
-      </c>
-      <c r="F12" t="n">
-        <v>4335</v>
-      </c>
-      <c r="G12" t="n">
-        <v>13134</v>
-      </c>
+          <t>other income , net</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
       <c r="H12" t="n">
-        <v>17469</v>
+        <v>1416</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -4011,23 +3995,23 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>general and administrative</t>
+          <t>research and development</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1166</v>
+        <v>3574</v>
       </c>
       <c r="E13" t="n">
-        <v>1109</v>
+        <v>3504</v>
       </c>
       <c r="F13" t="n">
-        <v>1208</v>
+        <v>3715</v>
       </c>
       <c r="G13" t="n">
-        <v>3546</v>
+        <v>11011</v>
       </c>
       <c r="H13" t="n">
-        <v>4754</v>
+        <v>14726</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -4121,15 +4105,23 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>impairment and restructuring</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
+          <t>sales and marketing</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>3812</v>
+      </c>
+      <c r="E14" t="n">
+        <v>4562</v>
+      </c>
+      <c r="F14" t="n">
+        <v>4335</v>
+      </c>
+      <c r="G14" t="n">
+        <v>13134</v>
+      </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>17469</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -4187,23 +4179,23 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>operating income</t>
+          <t>general and administrative</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>7708</v>
+        <v>1166</v>
       </c>
       <c r="E15" t="n">
-        <v>8679</v>
+        <v>1109</v>
       </c>
       <c r="F15" t="n">
-        <v>8292</v>
+        <v>1208</v>
       </c>
       <c r="G15" t="n">
-        <v>26766</v>
+        <v>3546</v>
       </c>
       <c r="H15" t="n">
-        <v>35058</v>
+        <v>4754</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -4297,15 +4289,23 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>other income , net</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
+          <t>operating income</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>7708</v>
+      </c>
+      <c r="E16" t="n">
+        <v>8679</v>
+      </c>
+      <c r="F16" t="n">
+        <v>8292</v>
+      </c>
+      <c r="G16" t="n">
+        <v>26766</v>
+      </c>
       <c r="H16" t="n">
-        <v>1416</v>
+        <v>35058</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -5045,7 +5045,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>weighted average shares outstanding:</t>
+          <t>product</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
@@ -5135,24 +5135,14 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>basic</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>7708</v>
-      </c>
-      <c r="E25" t="n">
-        <v>7710</v>
-      </c>
-      <c r="F25" t="n">
-        <v>7698</v>
-      </c>
-      <c r="G25" t="n">
-        <v>2</v>
-      </c>
-      <c r="H25" t="n">
-        <v>7700</v>
-      </c>
+          <t>weighted average shares outstanding:</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr">
         <is>
           <t>revenue</t>
@@ -5245,23 +5235,15 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>diluted</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>7799</v>
-      </c>
-      <c r="E26" t="n">
-        <v>7710</v>
-      </c>
-      <c r="F26" t="n">
-        <v>7794</v>
-      </c>
-      <c r="G26" t="n">
-        <v>0</v>
-      </c>
+          <t>revenue</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
       <c r="H26" t="n">
-        <v>7794</v>
+        <v>64497</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
@@ -5307,23 +5289,23 @@
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr">
         <is>
-          <t>cash dividends declared per common share</t>
+          <t>basic</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.42</v>
+        <v>7708</v>
       </c>
       <c r="E27" t="n">
-        <v>0.42</v>
+        <v>7710</v>
       </c>
       <c r="F27" t="n">
-        <v>0.42</v>
+        <v>7698</v>
       </c>
       <c r="G27" t="n">
-        <v>1.26</v>
+        <v>2</v>
       </c>
       <c r="H27" t="n">
-        <v>1.68</v>
+        <v>7700</v>
       </c>
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
@@ -5355,14 +5337,16 @@
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
-          <t>product</t>
+          <t>cost of revenue</t>
         </is>
       </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
+      <c r="H28" t="n">
+        <v>15420</v>
+      </c>
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
@@ -5393,15 +5377,23 @@
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
-          <t>revenue</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
+          <t>diluted</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>7799</v>
+      </c>
+      <c r="E29" t="n">
+        <v>7710</v>
+      </c>
+      <c r="F29" t="n">
+        <v>7794</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
       <c r="H29" t="n">
-        <v>64497</v>
+        <v>7794</v>
       </c>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
@@ -5433,16 +5425,14 @@
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr">
         <is>
-          <t>cost of revenue</t>
+          <t>service and other</t>
         </is>
       </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
-      <c r="H30" t="n">
-        <v>15420</v>
-      </c>
+      <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
@@ -5473,14 +5463,24 @@
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr">
         <is>
-          <t>service and other</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
+          <t>cash dividends declared per common share</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="H31" t="n">
+        <v>1.68</v>
+      </c>
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr"/>

</xml_diff>